<commit_message>
update title page and coauthors
</commit_message>
<xml_diff>
--- a/ms/coautores_MS wildlifefatalModelling.xlsx
+++ b/ms/coautores_MS wildlifefatalModelling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62d8cbee2955d9a6/PROJETOS/Fogo2020_RPPN Sesc/MS_WildfireMortalModelling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62d8cbee2955d9a6/PROJETOS/Fogo2020_RPPN Sesc/MS_Mortalities_Pantanal2020/ms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="259" documentId="11_92485C45C1F39E42E268565A893E8C18510380CC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2612E79D-9B74-4CFD-974C-096984886C61}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="11_92485C45C1F39E42E268565A893E8C18510380CC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40CD6A75-F2B9-40D4-9B45-439130E69345}"/>
   <bookViews>
-    <workbookView xWindow="29490" yWindow="-1620" windowWidth="14580" windowHeight="18285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28830" yWindow="5655" windowWidth="15960" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="co-autores" sheetId="1" r:id="rId1"/>
@@ -769,15 +769,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="42.85546875" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1"/>
-    <col min="4" max="4" width="185.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="185.85546875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="32.140625" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="7" width="39.28515625" customWidth="1"/>
@@ -826,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45.75">
+    <row r="3" spans="1:7" ht="45">
       <c r="A3">
         <v>3</v>
       </c>
@@ -865,7 +865,7 @@
       <c r="E4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -888,7 +888,7 @@
       <c r="E5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="G5" t="s">
@@ -934,7 +934,7 @@
       <c r="E7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -964,7 +964,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30.75">
+    <row r="9" spans="1:7" ht="45">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1095,7 +1095,7 @@
       <c r="E14" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="5" t="s">
         <v>71</v>
       </c>
       <c r="G14" t="s">
@@ -1205,6 +1205,10 @@
     <hyperlink ref="G13" r:id="rId10" xr:uid="{88945AEA-D4F0-CA4C-A358-CE89DC4AE7A0}"/>
     <hyperlink ref="F18" r:id="rId11" xr:uid="{1947A397-A5CC-4654-BEEF-D2F9AFAD3EC2}"/>
     <hyperlink ref="F17" r:id="rId12" xr:uid="{24E285C6-F423-4759-9A23-E79726EEA05B}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{6B69576C-BBB1-46B1-9C06-9AF7061B4A95}"/>
+    <hyperlink ref="F14" r:id="rId14" xr:uid="{8F9E4421-93F8-4D9A-B9DE-7256A9B628E1}"/>
+    <hyperlink ref="F5" r:id="rId15" xr:uid="{E9160116-93EB-41E7-8A5D-151B72E712E7}"/>
+    <hyperlink ref="F7" r:id="rId16" xr:uid="{45938BF1-473D-482F-B297-F4A0BFF471F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>